<commit_message>
finalized q5 and trend data
</commit_message>
<xml_diff>
--- a/Q5_trends.xlsx
+++ b/Q5_trends.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokey\Documents\NSS\Projects\lahman-baseball-data-space-jam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NSS\Projects\lahman-baseball-data-space-jam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8158E8-5EEC-4CC6-90BD-DF484D85A7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5909252-DA73-4EDE-9128-D15353468B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q5_trends" sheetId="1" r:id="rId1"/>
@@ -708,34 +708,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31</c:v>
+                  <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>10.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.53</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,7 +949,7 @@
         <c:axId val="1650031216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.9"/>
+          <c:max val="16"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1221,34 +1221,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.04</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.06</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.06</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.06</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.08</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2951,12 +2951,12 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2967,114 +2967,114 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1920</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>5.6</v>
       </c>
       <c r="C2">
-        <v>0.04</v>
+        <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1930</v>
       </c>
       <c r="B3">
-        <v>0.28999999999999998</v>
+        <v>6.6</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1940</v>
       </c>
       <c r="B4">
-        <v>0.31</v>
+        <v>7.1</v>
       </c>
       <c r="C4">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1950</v>
       </c>
       <c r="B5">
-        <v>0.35</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C5">
-        <v>7.0000000000000007E-2</v>
+        <v>1.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1960</v>
       </c>
       <c r="B6">
-        <v>0.45</v>
+        <v>11.4</v>
       </c>
       <c r="C6">
-        <v>0.06</v>
+        <v>1.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1970</v>
       </c>
       <c r="B7">
-        <v>0.4</v>
+        <v>10.3</v>
       </c>
       <c r="C7">
-        <v>0.06</v>
+        <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1980</v>
       </c>
       <c r="B8">
-        <v>0.4</v>
+        <v>10.7</v>
       </c>
       <c r="C8">
-        <v>0.06</v>
+        <v>1.6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1990</v>
       </c>
       <c r="B9">
-        <v>0.44</v>
+        <v>12.3</v>
       </c>
       <c r="C9">
-        <v>7.0000000000000007E-2</v>
+        <v>1.9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2000</v>
       </c>
       <c r="B10">
-        <v>0.46</v>
+        <v>13.1</v>
       </c>
       <c r="C10">
-        <v>0.08</v>
+        <v>2.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2010</v>
       </c>
       <c r="B11">
-        <v>0.53</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>7.0000000000000007E-2</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>